<commit_message>
Admins-Responsiveness Related Bugs have been reported
</commit_message>
<xml_diff>
--- a/docs/qa_guides/Frontend_Bugs_and_Refactoring_Template(AutoRecovered).xlsx
+++ b/docs/qa_guides/Frontend_Bugs_and_Refactoring_Template(AutoRecovered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semesters\FYP\Development\Philbox\docs\qa_guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{9264F107-4CA5-4FFB-AD35-74F934E2A131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3630EC70-E70D-4AFB-9464-F3C81545F489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,11 @@
     <sheet name="Refactoring Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="185">
   <si>
     <t>Bug ID</t>
   </si>
@@ -31,9 +30,6 @@
   </si>
   <si>
     <t>Environment (Browser/Device)</t>
-  </si>
-  <si>
-    <t>Bug Title</t>
   </si>
   <si>
     <t>Description</t>
@@ -361,6 +357,338 @@
   </si>
   <si>
     <t>2nd Feb, 2026</t>
+  </si>
+  <si>
+    <t>A-009</t>
+  </si>
+  <si>
+    <t>All Admins Page</t>
+  </si>
+  <si>
+    <t>The numbers inside the 3 divs (above the Branch admins cards are getting outside those divs on small screens</t>
+  </si>
+  <si>
+    <t>update tailwind classes</t>
+  </si>
+  <si>
+    <t>on small screens make those 3 divs to be vertically aligned (one over another) instead of horizontal allignment</t>
+  </si>
+  <si>
+    <t>those 3 divs are horizontally alligned</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\all-admins-page-icons.png</t>
+  </si>
+  <si>
+    <t>A-010</t>
+  </si>
+  <si>
+    <t>The buttons on admins cards are justified to end. For smaller screens make them justify center or the best choice is justify between</t>
+  </si>
+  <si>
+    <t>justify between</t>
+  </si>
+  <si>
+    <t>justify end</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\admins-cards-buttons.png</t>
+  </si>
+  <si>
+    <t>A-011</t>
+  </si>
+  <si>
+    <t>Add New Admin Page</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The font size of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add New Admin </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is too large on small screens</t>
+    </r>
+  </si>
+  <si>
+    <t>it’s a bit large</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\add-new-admin.png</t>
+  </si>
+  <si>
+    <t>A-012</t>
+  </si>
+  <si>
+    <t>This page is irresponsive may be because of form</t>
+  </si>
+  <si>
+    <t>it must be responsive</t>
+  </si>
+  <si>
+    <t>irresponsive</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Staff-Management-Salespersons-Page.png</t>
+  </si>
+  <si>
+    <t>Salespersons Page in Staff Management</t>
+  </si>
+  <si>
+    <t>A-013</t>
+  </si>
+  <si>
+    <t>SideBar on Salespersons Page in Staff Management</t>
+  </si>
+  <si>
+    <t>The sidebar on this page is irresponsive</t>
+  </si>
+  <si>
+    <t>update tailwindd classes</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Staff-Management-SideBar-Salesperson.png</t>
+  </si>
+  <si>
+    <t>A-014</t>
+  </si>
+  <si>
+    <t>Staff Management Add New Salespersons Page</t>
+  </si>
+  <si>
+    <t>The font size of Add New Salesperson is too large on small screens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">font size of heading Add New Salesperson is too much large </t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Add-new-Salesperson.png</t>
+  </si>
+  <si>
+    <t>A-015</t>
+  </si>
+  <si>
+    <t>Doctors Applications Page</t>
+  </si>
+  <si>
+    <t>The Doctors Applications Page is not Responsive</t>
+  </si>
+  <si>
+    <t>responsive</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Doctors-Applications.png</t>
+  </si>
+  <si>
+    <t>A-016</t>
+  </si>
+  <si>
+    <t>Task Management Page</t>
+  </si>
+  <si>
+    <t>This page is not responsive</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\task-management.png</t>
+  </si>
+  <si>
+    <t>A-017</t>
+  </si>
+  <si>
+    <t>As per the requirements mentioned in the document we are required to show a proper task management board (like jira)</t>
+  </si>
+  <si>
+    <t>update the ui of this page and provide a board</t>
+  </si>
+  <si>
+    <t>tasks are shown in table</t>
+  </si>
+  <si>
+    <t>tasks must be shown in a board</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\tasks-table.png</t>
+  </si>
+  <si>
+    <t>A-018</t>
+  </si>
+  <si>
+    <t>Customer Management Page</t>
+  </si>
+  <si>
+    <t>The customer management page is irresponsive</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Customer Management Page.png</t>
+  </si>
+  <si>
+    <t>A-019</t>
+  </si>
+  <si>
+    <t>Revenue Analytics Page</t>
+  </si>
+  <si>
+    <t>The revnue analytics page is not responsive</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\revenue-analytics.png</t>
+  </si>
+  <si>
+    <t>A-020</t>
+  </si>
+  <si>
+    <t>There is a div on revenue-analytics-page that is showing a loading card a circle in center and a rectangle at the top left</t>
+  </si>
+  <si>
+    <t>remove it</t>
+  </si>
+  <si>
+    <t>after loading it should be removed</t>
+  </si>
+  <si>
+    <t>its visible even after loading</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\revenue-analytics-waste-card.png</t>
+  </si>
+  <si>
+    <t>A-021</t>
+  </si>
+  <si>
+    <t>User Engagement Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This page is irresponsive </t>
+  </si>
+  <si>
+    <t>bugs\screenshots\User-Engagement-Page.png</t>
+  </si>
+  <si>
+    <t>A-022</t>
+  </si>
+  <si>
+    <t>Activity Logs Page</t>
+  </si>
+  <si>
+    <t>This page is irresponasive</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Activity Logs Page.png</t>
+  </si>
+  <si>
+    <t>Bug Category</t>
+  </si>
+  <si>
+    <t>A-023</t>
+  </si>
+  <si>
+    <t>Feedback and Complaints Analytics Page</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Feedback-Complaints-Analytics.png</t>
+  </si>
+  <si>
+    <t>A-024</t>
+  </si>
+  <si>
+    <t>Appointments Analytics Page</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Appointment-Analytics-Page.png</t>
+  </si>
+  <si>
+    <t>A-025</t>
+  </si>
+  <si>
+    <t>Admin Dashboard Footer</t>
+  </si>
+  <si>
+    <t>this is too much concise footer. Provide a professional footer</t>
+  </si>
+  <si>
+    <t>add some content in it</t>
+  </si>
+  <si>
+    <t>detailed footer</t>
+  </si>
+  <si>
+    <t>single line footer</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\admin-Footer.png</t>
+  </si>
+  <si>
+    <t>A-026</t>
+  </si>
+  <si>
+    <t>Roles And Permissions Page</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Roles-Permissions-Admin.png</t>
+  </si>
+  <si>
+    <t>A-027</t>
+  </si>
+  <si>
+    <t>Notifications Page</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Notifications-Page.png</t>
+  </si>
+  <si>
+    <t>A-028</t>
+  </si>
+  <si>
+    <t>Settings Page</t>
+  </si>
+  <si>
+    <t>The 2fa enable button on small screen is too bad because of irresponsiveness</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Admin-Settings.png</t>
+  </si>
+  <si>
+    <t>A-029</t>
+  </si>
+  <si>
+    <t>Admin Dashboard Searchbar</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>the search bar must allow admin to search about any of the features which we are providing on dashboard. For example if admin searches about branches the search bar must show all the branch related activities that admin can do in a dropdown</t>
+  </si>
+  <si>
+    <t>implement this functionality on frontend</t>
+  </si>
+  <si>
+    <t>search bar must provide correct response on admins search</t>
+  </si>
+  <si>
+    <t>search bar is providing nothing</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Search-Bar-Admin-Dashboard.png</t>
   </si>
 </sst>
 </file>
@@ -728,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,395 +1083,1319 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
       <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
       <c r="M2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
       <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>58</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>59</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>64</v>
       </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>65</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>70</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>74</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L16" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" t="s">
         <v>79</v>
       </c>
-      <c r="I9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L18" t="s">
         <v>81</v>
       </c>
-      <c r="L9" t="s">
-        <v>82</v>
-      </c>
-      <c r="M9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O9" t="s">
-        <v>42</v>
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L21" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L22" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L23" t="s">
+        <v>81</v>
+      </c>
+      <c r="M23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L24" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" t="s">
+        <v>39</v>
+      </c>
+      <c r="O24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L25" t="s">
+        <v>81</v>
+      </c>
+      <c r="M25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L26" t="s">
+        <v>81</v>
+      </c>
+      <c r="M26" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" t="s">
+        <v>103</v>
+      </c>
+      <c r="I27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L28" t="s">
+        <v>81</v>
+      </c>
+      <c r="M28" t="s">
+        <v>39</v>
+      </c>
+      <c r="O28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L29" t="s">
+        <v>81</v>
+      </c>
+      <c r="M29" t="s">
+        <v>39</v>
+      </c>
+      <c r="O29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>179</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>181</v>
+      </c>
+      <c r="G30" t="s">
+        <v>182</v>
+      </c>
+      <c r="H30" t="s">
+        <v>183</v>
+      </c>
+      <c r="I30" t="s">
+        <v>79</v>
+      </c>
+      <c r="J30" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L30" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" t="s">
+        <v>39</v>
+      </c>
+      <c r="O30" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1156,8 +2408,30 @@
     <hyperlink ref="K7" r:id="rId6" xr:uid="{94DA2FC6-9DFB-403B-A3A7-CFD461513103}"/>
     <hyperlink ref="K8" r:id="rId7" xr:uid="{14582111-A968-45D4-B6D2-C94740349ED8}"/>
     <hyperlink ref="K9" r:id="rId8" xr:uid="{6BE5CE4A-D286-4436-BDE9-DED0CA1E07CD}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{7A907286-7EC9-4EBC-8109-8C3AEABE46C1}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{F003A764-DD2C-48AE-AA2B-5FDC676B52CA}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{197BD63F-5C46-4C65-95E6-8F212A12F1BB}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{8ADA24B1-E080-43C5-8818-19669AD565E3}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{616B67D1-FA6C-4571-8949-458999B65265}"/>
+    <hyperlink ref="K15" r:id="rId14" xr:uid="{B1D7A3A8-6564-40D6-90EF-8B1E24AA58CD}"/>
+    <hyperlink ref="K16" r:id="rId15" xr:uid="{22F7946B-5F66-4490-8435-8C76D361D22A}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{30DEDCAF-4C48-4C8B-AC06-05AE004F171E}"/>
+    <hyperlink ref="K18" r:id="rId17" xr:uid="{F12415D8-F3D7-48C4-A2BB-7F0907571554}"/>
+    <hyperlink ref="K19" r:id="rId18" xr:uid="{A5322380-8B47-48A1-9972-E394189BE00F}"/>
+    <hyperlink ref="K20" r:id="rId19" xr:uid="{BACFB6F0-4C7B-4313-9914-2FF8E957498F}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{910011FF-69F8-4F6A-A1BE-8E2FBC157A82}"/>
+    <hyperlink ref="K22" r:id="rId21" xr:uid="{1F2A2B94-FB32-4BC3-BC7B-E60BF7B9A2D7}"/>
+    <hyperlink ref="K23" r:id="rId22" xr:uid="{864C5C61-0DC5-4047-A13D-F279773D464D}"/>
+    <hyperlink ref="K24" r:id="rId23" xr:uid="{B5BB10C9-3B9F-4EBB-80AD-5D2BAC6529B3}"/>
+    <hyperlink ref="K25" r:id="rId24" xr:uid="{927C5EFD-1BB5-44DD-806C-FEE7BE917890}"/>
+    <hyperlink ref="K26" r:id="rId25" xr:uid="{2E681D55-F197-47C6-B29B-DE0D34CBD115}"/>
+    <hyperlink ref="K27" r:id="rId26" xr:uid="{8FE57E8C-43D0-4A5C-9AD9-36656E7968C2}"/>
+    <hyperlink ref="K28" r:id="rId27" xr:uid="{9FD8B77F-3E5B-484F-8EED-A77808213E74}"/>
+    <hyperlink ref="K29" r:id="rId28" xr:uid="{67313903-D8A0-443A-AFE7-B447AC64FD2A}"/>
+    <hyperlink ref="K30" r:id="rId29" xr:uid="{9DD8C582-2FA1-4435-BD88-6642F9FE20B9}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
@@ -1174,31 +2448,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug report in progress
</commit_message>
<xml_diff>
--- a/docs/qa_guides/Frontend_Bugs_and_Refactoring_Template(AutoRecovered).xlsx
+++ b/docs/qa_guides/Frontend_Bugs_and_Refactoring_Template(AutoRecovered).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semesters\FYP\Development\Philbox\docs\qa_guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3630EC70-E70D-4AFB-9464-F3C81545F489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1457A36-E1F2-4313-A705-645094E0B4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend Bugs" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="221">
   <si>
     <t>Bug ID</t>
   </si>
@@ -689,6 +689,114 @@
   </si>
   <si>
     <t>bugs\screenshots\Search-Bar-Admin-Dashboard.png</t>
+  </si>
+  <si>
+    <t>A-030</t>
+  </si>
+  <si>
+    <t>Admin Landing Page</t>
+  </si>
+  <si>
+    <t>The Active Users and Response Time cards on Admin Setting image must not be visible on small screens</t>
+  </si>
+  <si>
+    <t>either remove them or make some change for maing it responsive</t>
+  </si>
+  <si>
+    <t>those 2 cards must be static beneath the setting image instead of floating on it</t>
+  </si>
+  <si>
+    <t>those 2 cards are floating on the setting image</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Landing-Page-Admin.png</t>
+  </si>
+  <si>
+    <t>A-031</t>
+  </si>
+  <si>
+    <t>Exagerated Lies</t>
+  </si>
+  <si>
+    <t>Stop presenting lies</t>
+  </si>
+  <si>
+    <t>remove ip whitelisting, automatic logout</t>
+  </si>
+  <si>
+    <t>correct info</t>
+  </si>
+  <si>
+    <t>incorrect info</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\landing-admin-details.png</t>
+  </si>
+  <si>
+    <t>C-001</t>
+  </si>
+  <si>
+    <t>Though we have a single landing page for both customers and doctors it does not mean we are free to place any button anywhere. See how bad UX will be when a customer will see this login as doctor button. Just show a single login button on the top of the page at th very right top corner. and remove get started button from right top corner. further in hero section just show a get started button. remove login as doctor button.</t>
+  </si>
+  <si>
+    <t>update this landing page</t>
+  </si>
+  <si>
+    <t>as mentioned in description</t>
+  </si>
+  <si>
+    <t>current wrong state</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\customer-doctor-landing.png</t>
+  </si>
+  <si>
+    <t>C-002</t>
+  </si>
+  <si>
+    <t>Customer Doctor Landing Page</t>
+  </si>
+  <si>
+    <t>Remove buttons in for doctors dection and make the heading for doctors more prominent</t>
+  </si>
+  <si>
+    <t>same as of description</t>
+  </si>
+  <si>
+    <t>just details</t>
+  </si>
+  <si>
+    <t>buttons are also shown</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\doctors-landing.png</t>
+  </si>
+  <si>
+    <t>C-003</t>
+  </si>
+  <si>
+    <t>Wrong date in footer</t>
+  </si>
+  <si>
+    <t>instead of hardcoding the date use Date object and get year from that object</t>
+  </si>
+  <si>
+    <t>current year</t>
+  </si>
+  <si>
+    <t>hard coded year</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\landing date.png</t>
+  </si>
+  <si>
+    <t>C-004</t>
+  </si>
+  <si>
+    <t>philbox icons size is too large</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\landing-doctor-foter-icon.png</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,6 +2503,270 @@
         <v>39</v>
       </c>
       <c r="O30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>187</v>
+      </c>
+      <c r="F31" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H31" t="s">
+        <v>190</v>
+      </c>
+      <c r="I31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L31" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" t="s">
+        <v>39</v>
+      </c>
+      <c r="O31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>193</v>
+      </c>
+      <c r="E32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" t="s">
+        <v>195</v>
+      </c>
+      <c r="G32" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" t="s">
+        <v>197</v>
+      </c>
+      <c r="I32" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L32" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+      <c r="O32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G33" t="s">
+        <v>202</v>
+      </c>
+      <c r="H33" t="s">
+        <v>203</v>
+      </c>
+      <c r="I33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L33" t="s">
+        <v>81</v>
+      </c>
+      <c r="M33" t="s">
+        <v>39</v>
+      </c>
+      <c r="O33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" t="s">
+        <v>208</v>
+      </c>
+      <c r="G34" t="s">
+        <v>209</v>
+      </c>
+      <c r="H34" t="s">
+        <v>210</v>
+      </c>
+      <c r="I34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L34" t="s">
+        <v>81</v>
+      </c>
+      <c r="M34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>179</v>
+      </c>
+      <c r="E35" t="s">
+        <v>213</v>
+      </c>
+      <c r="F35" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" t="s">
+        <v>216</v>
+      </c>
+      <c r="I35" t="s">
+        <v>93</v>
+      </c>
+      <c r="J35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L35" t="s">
+        <v>81</v>
+      </c>
+      <c r="M35" t="s">
+        <v>39</v>
+      </c>
+      <c r="O35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>219</v>
+      </c>
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="L36" t="s">
+        <v>81</v>
+      </c>
+      <c r="M36" t="s">
+        <v>39</v>
+      </c>
+      <c r="O36" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2429,9 +2801,15 @@
     <hyperlink ref="K28" r:id="rId27" xr:uid="{9FD8B77F-3E5B-484F-8EED-A77808213E74}"/>
     <hyperlink ref="K29" r:id="rId28" xr:uid="{67313903-D8A0-443A-AFE7-B447AC64FD2A}"/>
     <hyperlink ref="K30" r:id="rId29" xr:uid="{9DD8C582-2FA1-4435-BD88-6642F9FE20B9}"/>
+    <hyperlink ref="K31" r:id="rId30" xr:uid="{C4C66B39-44C0-4E72-9014-CEC2DAD19830}"/>
+    <hyperlink ref="K32" r:id="rId31" xr:uid="{00CB6BDC-13AD-40C8-8665-23EF166075A8}"/>
+    <hyperlink ref="K33" r:id="rId32" xr:uid="{597C8937-3F9A-47D3-8B39-93B3A9709861}"/>
+    <hyperlink ref="K34" r:id="rId33" xr:uid="{618B6ADE-B453-4A05-91D0-6A77F66575C2}"/>
+    <hyperlink ref="K35" r:id="rId34" xr:uid="{1C3C2FF2-5376-42EF-93F4-40745ADD3F65}"/>
+    <hyperlink ref="K36" r:id="rId35" xr:uid="{ABBA607B-E98F-4ACC-8057-5D87EC06529B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
doctor and customer bug report updated, More bugs are added
</commit_message>
<xml_diff>
--- a/docs/qa_guides/Frontend_Bugs_and_Refactoring_Template(AutoRecovered).xlsx
+++ b/docs/qa_guides/Frontend_Bugs_and_Refactoring_Template(AutoRecovered).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semesters\FYP\Development\Philbox\docs\qa_guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\fyp\Philbox\docs\qa_guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058E70EB-A75D-4397-9106-2E25687FBEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21E13F7-5A6A-4B04-8C60-9F6A8D6D5207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend Bugs" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="292">
   <si>
     <t>Bug ID</t>
   </si>
@@ -825,12 +825,198 @@
   <si>
     <t>20nd Feb, 2026</t>
   </si>
+  <si>
+    <t>C-006</t>
+  </si>
+  <si>
+    <t>Notification drop down on customer dashboard</t>
+  </si>
+  <si>
+    <t>The minimum screen is 280 and the notification drop down goes out of sight</t>
+  </si>
+  <si>
+    <t>Make it visible and responsive</t>
+  </si>
+  <si>
+    <t>22nd Feb,2026</t>
+  </si>
+  <si>
+    <t>23rd Feb, 2026</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\customer-page-notification-dropdorn.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Dashboard cards </t>
+  </si>
+  <si>
+    <t>The minimum screen is 280 and the cards icon goes out of cards.</t>
+  </si>
+  <si>
+    <t>Make it with within the cards</t>
+  </si>
+  <si>
+    <t>Must be adjusted according to the cards size.</t>
+  </si>
+  <si>
+    <t>23rd Feb,2026</t>
+  </si>
+  <si>
+    <t>24th Feb, 2026</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\customer-Dasbboard-cards.PNG</t>
+  </si>
+  <si>
+    <t>C-008</t>
+  </si>
+  <si>
+    <t>C-007</t>
+  </si>
+  <si>
+    <t>Customer Medicine detail page</t>
+  </si>
+  <si>
+    <t>The minimum screen is 280 and the buy now and cadd to cart buttons and other things goes out of the card</t>
+  </si>
+  <si>
+    <t>Make it responsive</t>
+  </si>
+  <si>
+    <t>Must be adjusted according to the card size</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\customer-medicine-details-page.PNG</t>
+  </si>
+  <si>
+    <t>24th Feb,2026</t>
+  </si>
+  <si>
+    <t>25th Feb, 2026</t>
+  </si>
+  <si>
+    <t>C-009</t>
+  </si>
+  <si>
+    <t>Customer order detail page</t>
+  </si>
+  <si>
+    <t>the minimum screen is 280 and the card size miss matched</t>
+  </si>
+  <si>
+    <t>make it responsive</t>
+  </si>
+  <si>
+    <t>Must be adjusted dso that in small screen all cards have same width</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Customer-order-detail-page.PNG</t>
+  </si>
+  <si>
+    <t>23th Feb,2026</t>
+  </si>
+  <si>
+    <t>C-0010</t>
+  </si>
+  <si>
+    <t>Customer Appointment page botton size</t>
+  </si>
+  <si>
+    <t>The buttons on the appointment cards are of unequal lengths make their width equal when the are in small screen</t>
+  </si>
+  <si>
+    <t>make them of equal width</t>
+  </si>
+  <si>
+    <t>Must be adjusted so that in small screen they seem to be of equal width</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\customer-appointment-page-button size.PNG</t>
+  </si>
+  <si>
+    <t>C-0011</t>
+  </si>
+  <si>
+    <t>Customer book Appointment cards and timeline</t>
+  </si>
+  <si>
+    <t>the min screen size is 280 and the cards of search bar and appointment width mismatched and the time line also goes out of sight</t>
+  </si>
+  <si>
+    <t>must be adjusted to equal widths also time line should be visible</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\Customer-book-appointment responsiveness.PNG</t>
+  </si>
+  <si>
+    <t>C-0012</t>
+  </si>
+  <si>
+    <t>Customer Profile page security tab</t>
+  </si>
+  <si>
+    <t>the min screen size is 280 and the button goes out of the card</t>
+  </si>
+  <si>
+    <t>when the screen size is small the button should be inside the card</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\customer-profile-security-tab.PNG</t>
+  </si>
+  <si>
+    <t>D-001</t>
+  </si>
+  <si>
+    <t>Doctor Registration page logo</t>
+  </si>
+  <si>
+    <t>Ux</t>
+  </si>
+  <si>
+    <t>the logo of vite is shown instead of philbox logo</t>
+  </si>
+  <si>
+    <t>adjust the logo of philbox</t>
+  </si>
+  <si>
+    <t>must show the logo of philbox</t>
+  </si>
+  <si>
+    <t>bugs\screenshots\doctor-registration-page.PNG</t>
+  </si>
+  <si>
+    <t>D-002</t>
+  </si>
+  <si>
+    <t>Doctor login page logo</t>
+  </si>
+  <si>
+    <t>D-003</t>
+  </si>
+  <si>
+    <t>Doctor complete profile</t>
+  </si>
+  <si>
+    <t>ux</t>
+  </si>
+  <si>
+    <t>D-004</t>
+  </si>
+  <si>
+    <t>password and confirm password text bxes size mismatched</t>
+  </si>
+  <si>
+    <t>must be adjusted</t>
+  </si>
+  <si>
+    <t>the size of the textboxes must be responsive and well managed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,6 +1044,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1191,23 +1383,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35:O48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="13" width="25" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1301,7 +1493,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1537,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1389,7 +1581,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1433,7 +1625,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1477,7 +1669,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1521,7 +1713,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1565,7 +1757,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1609,7 +1801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -1653,7 +1845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1697,7 +1889,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -1741,7 +1933,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1785,7 +1977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -1829,7 +2021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -1873,7 +2065,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -1917,7 +2109,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>121</v>
       </c>
@@ -1961,7 +2153,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -2005,7 +2197,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -2049,7 +2241,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>135</v>
       </c>
@@ -2093,7 +2285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -2137,7 +2329,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2181,7 +2373,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>149</v>
       </c>
@@ -2225,7 +2417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>154</v>
       </c>
@@ -2269,7 +2461,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -2313,7 +2505,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -2357,7 +2549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>167</v>
       </c>
@@ -2401,7 +2593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>170</v>
       </c>
@@ -2445,7 +2637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>173</v>
       </c>
@@ -2489,7 +2681,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>177</v>
       </c>
@@ -2533,7 +2725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -2577,7 +2769,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>192</v>
       </c>
@@ -2621,7 +2813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>199</v>
       </c>
@@ -2665,7 +2857,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>205</v>
       </c>
@@ -2709,7 +2901,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>212</v>
       </c>
@@ -2753,7 +2945,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>218</v>
       </c>
@@ -2797,7 +2989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>221</v>
       </c>
@@ -2837,8 +3029,496 @@
       <c r="M37" t="s">
         <v>228</v>
       </c>
+      <c r="O37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" t="s">
+        <v>231</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>232</v>
+      </c>
+      <c r="F38" t="s">
+        <v>233</v>
+      </c>
+      <c r="G38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>103</v>
+      </c>
+      <c r="I38" t="s">
+        <v>27</v>
+      </c>
+      <c r="J38" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L38" t="s">
+        <v>234</v>
+      </c>
+      <c r="M38" t="s">
+        <v>235</v>
+      </c>
+      <c r="O38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" t="s">
+        <v>239</v>
+      </c>
+      <c r="G39" t="s">
+        <v>240</v>
+      </c>
+      <c r="H39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L39" t="s">
+        <v>241</v>
+      </c>
+      <c r="M39" t="s">
+        <v>242</v>
+      </c>
+      <c r="O39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>244</v>
+      </c>
+      <c r="B40" t="s">
+        <v>246</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>247</v>
+      </c>
+      <c r="F40" t="s">
+        <v>248</v>
+      </c>
+      <c r="G40" t="s">
+        <v>249</v>
+      </c>
+      <c r="H40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I40" t="s">
+        <v>27</v>
+      </c>
+      <c r="J40" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L40" t="s">
+        <v>251</v>
+      </c>
+      <c r="M40" t="s">
+        <v>252</v>
+      </c>
+      <c r="O40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>253</v>
+      </c>
+      <c r="B41" t="s">
+        <v>254</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>255</v>
+      </c>
+      <c r="F41" t="s">
+        <v>256</v>
+      </c>
+      <c r="G41" t="s">
+        <v>257</v>
+      </c>
+      <c r="H41" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J41" t="s">
+        <v>28</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L41" t="s">
+        <v>259</v>
+      </c>
+      <c r="M41" t="s">
+        <v>242</v>
+      </c>
+      <c r="O41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>260</v>
+      </c>
+      <c r="B42" t="s">
+        <v>261</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>262</v>
+      </c>
+      <c r="F42" t="s">
+        <v>263</v>
+      </c>
+      <c r="G42" t="s">
+        <v>264</v>
+      </c>
+      <c r="H42" t="s">
+        <v>103</v>
+      </c>
+      <c r="I42" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" t="s">
+        <v>28</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L42" t="s">
+        <v>259</v>
+      </c>
+      <c r="M42" t="s">
+        <v>242</v>
+      </c>
+      <c r="O42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>266</v>
+      </c>
+      <c r="B43" t="s">
+        <v>267</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>268</v>
+      </c>
+      <c r="F43" t="s">
+        <v>233</v>
+      </c>
+      <c r="G43" t="s">
+        <v>269</v>
+      </c>
+      <c r="H43" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L43" t="s">
+        <v>228</v>
+      </c>
+      <c r="M43" t="s">
+        <v>235</v>
+      </c>
+      <c r="O43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" t="s">
+        <v>272</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" t="s">
+        <v>273</v>
+      </c>
+      <c r="F44" t="s">
+        <v>256</v>
+      </c>
+      <c r="G44" t="s">
+        <v>274</v>
+      </c>
+      <c r="H44" t="s">
+        <v>103</v>
+      </c>
+      <c r="I44" t="s">
+        <v>27</v>
+      </c>
+      <c r="J44" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="L44" t="s">
+        <v>228</v>
+      </c>
+      <c r="M44" t="s">
+        <v>235</v>
+      </c>
+      <c r="O44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>276</v>
+      </c>
+      <c r="B45" t="s">
+        <v>277</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>278</v>
+      </c>
+      <c r="E45" t="s">
+        <v>279</v>
+      </c>
+      <c r="F45" t="s">
+        <v>280</v>
+      </c>
+      <c r="G45" t="s">
+        <v>281</v>
+      </c>
+      <c r="H45" t="s">
+        <v>226</v>
+      </c>
+      <c r="I45" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L45" t="s">
+        <v>228</v>
+      </c>
+      <c r="M45" t="s">
+        <v>235</v>
+      </c>
+      <c r="O45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>283</v>
+      </c>
+      <c r="B46" t="s">
+        <v>284</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>278</v>
+      </c>
+      <c r="E46" t="s">
+        <v>279</v>
+      </c>
+      <c r="F46" t="s">
+        <v>280</v>
+      </c>
+      <c r="G46" t="s">
+        <v>281</v>
+      </c>
+      <c r="H46" t="s">
+        <v>226</v>
+      </c>
+      <c r="I46" t="s">
+        <v>27</v>
+      </c>
+      <c r="J46" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L46" t="s">
+        <v>228</v>
+      </c>
+      <c r="M46" t="s">
+        <v>235</v>
+      </c>
+      <c r="O46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>285</v>
+      </c>
+      <c r="B47" t="s">
+        <v>286</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>287</v>
+      </c>
+      <c r="E47" t="s">
+        <v>279</v>
+      </c>
+      <c r="F47" t="s">
+        <v>280</v>
+      </c>
+      <c r="G47" t="s">
+        <v>281</v>
+      </c>
+      <c r="H47" t="s">
+        <v>226</v>
+      </c>
+      <c r="I47" t="s">
+        <v>27</v>
+      </c>
+      <c r="J47" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L47" t="s">
+        <v>228</v>
+      </c>
+      <c r="M47" t="s">
+        <v>235</v>
+      </c>
+      <c r="O47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>288</v>
+      </c>
+      <c r="B48" t="s">
+        <v>277</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" t="s">
+        <v>289</v>
+      </c>
+      <c r="F48" t="s">
+        <v>290</v>
+      </c>
+      <c r="G48" t="s">
+        <v>291</v>
+      </c>
+      <c r="H48" t="s">
+        <v>103</v>
+      </c>
+      <c r="I48" t="s">
+        <v>27</v>
+      </c>
+      <c r="J48" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L48" t="s">
+        <v>228</v>
+      </c>
+      <c r="M48" t="s">
+        <v>235</v>
+      </c>
+      <c r="O48" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" xr:uid="{7FC909CC-855C-47A2-BBD0-02C6480FC499}"/>
     <hyperlink ref="K3" r:id="rId2" xr:uid="{90EE97AC-5F97-4EC0-BC67-B270378001A0}"/>
@@ -2876,9 +3556,20 @@
     <hyperlink ref="K35" r:id="rId34" xr:uid="{1C3C2FF2-5376-42EF-93F4-40745ADD3F65}"/>
     <hyperlink ref="K36" r:id="rId35" xr:uid="{ABBA607B-E98F-4ACC-8057-5D87EC06529B}"/>
     <hyperlink ref="K37" r:id="rId36" xr:uid="{0CD417ED-9BF5-49B0-AC38-D13323646B78}"/>
+    <hyperlink ref="K38" r:id="rId37" xr:uid="{1330E8E9-4222-4D99-B471-A762D4C7BFAC}"/>
+    <hyperlink ref="K39" r:id="rId38" xr:uid="{50060393-6BFC-4AC4-AF68-1ACFE2D6968D}"/>
+    <hyperlink ref="K40" r:id="rId39" xr:uid="{635C6B86-5D7B-4A41-9D27-35645A2FCE58}"/>
+    <hyperlink ref="K41" r:id="rId40" xr:uid="{F22F0192-C6FD-4F79-A5BB-C783A98AA63F}"/>
+    <hyperlink ref="K42" r:id="rId41" xr:uid="{B53ED3B7-DF00-4A91-ACCE-D3E1DF8E0701}"/>
+    <hyperlink ref="K43" r:id="rId42" xr:uid="{8EFD53FB-6004-417A-BCAC-EDA986B42EBA}"/>
+    <hyperlink ref="K44" r:id="rId43" xr:uid="{C694EF44-24D5-4C81-B3F3-84EC2FA257A8}"/>
+    <hyperlink ref="K45" r:id="rId44" xr:uid="{F5F2046E-DAFA-4882-9C02-CD9B7B2205FB}"/>
+    <hyperlink ref="K46" r:id="rId45" xr:uid="{40DD3EE0-6088-4B53-8388-97F73D11D568}"/>
+    <hyperlink ref="K47" r:id="rId46" xr:uid="{40C4B132-A36D-4CCA-B235-B95BFDB53804}"/>
+    <hyperlink ref="K48" r:id="rId47" xr:uid="{10A9C74A-0A64-4B21-BC9B-D76B5DCE8C6F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId48"/>
 </worksheet>
 </file>
 
@@ -2888,12 +3579,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>

</xml_diff>